<commit_message>
ref #2 Final sprint configuration and documentation
- Added burndown
- Fixed error with tests
- Added evaluation
- Fixed tests
</commit_message>
<xml_diff>
--- a/docs/Sprint_B_Avaliacao_Interpares_3DC_G15.xlsx
+++ b/docs/Sprint_B_Avaliacao_Interpares_3DC_G15.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\LAPR5_3DC_G15\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454E6643-77BB-4D85-A5F9-3D2AF2F05C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1A5FAC8F-D342-4231-83F0-ACABC064ED8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Fill the cells with a blue background</t>
   </si>
@@ -102,7 +102,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -141,6 +141,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -156,7 +164,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -343,54 +351,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -436,18 +401,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="65" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="65" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -484,13 +444,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>400900</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>401260</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>6710</xdr:rowOff>
@@ -984,39 +944,39 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="7.875" customWidth="1"/>
-    <col min="8" max="8" width="8" customWidth="1"/>
+    <col min="4" max="6" width="7.875" customWidth="1"/>
+    <col min="7" max="7" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -1025,23 +985,22 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:8" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:11" ht="15.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="E8" s="25" t="s">
+      <c r="E8" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="27"/>
-    </row>
-    <row r="9" spans="1:8" ht="105.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F8" s="23"/>
+      <c r="G8" s="24"/>
+    </row>
+    <row r="9" spans="1:11" ht="105.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="15">
@@ -1056,12 +1015,10 @@
         <f>C12</f>
         <v>1150736</v>
       </c>
-      <c r="G9" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
+      <c r="K9" s="19"/>
+    </row>
+    <row r="10" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="20" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="12">
@@ -1074,15 +1031,11 @@
         <v>5</v>
       </c>
       <c r="F10" s="14">
-        <v>1</v>
-      </c>
-      <c r="G10" s="20">
-        <f>AVERAGE(D10:F10)</f>
-        <v>3.6666666666666665</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="24"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="21"/>
       <c r="C11" s="6">
         <v>1211503</v>
       </c>
@@ -1093,51 +1046,48 @@
         <v>5</v>
       </c>
       <c r="F11" s="10">
-        <v>1</v>
-      </c>
-      <c r="G11" s="21">
-        <f>AVERAGE(D11:F11)</f>
-        <v>3.6666666666666665</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="24"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="21"/>
       <c r="C12" s="6">
         <v>1150736</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="21" t="e">
-        <f>AVERAGE(D12:F12)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="6">
+        <v>5</v>
+      </c>
+      <c r="E12" s="7">
+        <v>5</v>
+      </c>
+      <c r="F12" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="1"/>
-      <c r="C13" s="18" t="s">
+      <c r="C13" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="18">
         <f>AVERAGE(D10:D12)</f>
         <v>5</v>
       </c>
-      <c r="E13" s="19">
+      <c r="E13" s="18">
         <f>AVERAGE(E10:E12)</f>
         <v>5</v>
       </c>
-      <c r="F13" s="19">
+      <c r="F13" s="18">
         <f>AVERAGE(F10:F12)</f>
-        <v>1</v>
-      </c>
-      <c r="G13" s="22"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>2.3333333333333335</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -1203,7 +1153,7 @@
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B10:B12"/>
-    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E8:G8"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:F12" xr:uid="{00000000-0002-0000-0000-000000000000}">

</xml_diff>